<commit_message>
Neue Daten - FW jetzt auch dabei
</commit_message>
<xml_diff>
--- a/data/voto_score_matrix.xlsx
+++ b/data/voto_score_matrix.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Gemeinsame Liste</t>
+          <t>Freie Wähler</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -484,15 +484,20 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
+          <t>Tierschutzpartei</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>UFFBASSE</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Volt</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>WGD</t>
         </is>
@@ -508,43 +513,46 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3963414634146342</v>
+        <v>0.4451219512195122</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6036585365853658</v>
+        <v>0.5914634146341463</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2926829268292683</v>
+        <v>0.3170731707317073</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2835365853658536</v>
+        <v>0.2347560975609756</v>
       </c>
       <c r="G2" t="n">
         <v>0.2774390243902439</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6310975609756098</v>
+        <v>0.6067073170731707</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2134146341463415</v>
+        <v>0.6128048780487805</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2134146341463415</v>
+        <v>0.2378048780487805</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4390243902439024</v>
+        <v>0.4024390243902439</v>
       </c>
       <c r="L2" t="n">
         <v>0.5335365853658537</v>
       </c>
       <c r="M2" t="n">
-        <v>0.423780487804878</v>
+        <v>0.225609756097561</v>
       </c>
       <c r="N2" t="n">
+        <v>0.4481707317073171</v>
+      </c>
+      <c r="O2" t="n">
         <v>0.2195121951219512</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.4695121951219512</v>
+      <c r="P2" t="n">
+        <v>0.4939024390243902</v>
       </c>
     </row>
     <row r="3">
@@ -554,7 +562,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3963414634146342</v>
+        <v>0.4451219512195122</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -575,7 +583,7 @@
         <v>0.5182926829268293</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6341463414634146</v>
+        <v>0.6280487804878049</v>
       </c>
       <c r="J3" t="n">
         <v>0.6371951219512195</v>
@@ -587,12 +595,15 @@
         <v>0.5945121951219512</v>
       </c>
       <c r="M3" t="n">
+        <v>0.6341463414634146</v>
+      </c>
+      <c r="N3" t="n">
         <v>0.6615853658536586</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.6097560975609756</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.6280487804878049</v>
       </c>
     </row>
@@ -603,7 +614,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6036585365853658</v>
+        <v>0.5914634146341463</v>
       </c>
       <c r="C4" t="n">
         <v>0.4329268292682927</v>
@@ -624,7 +635,7 @@
         <v>0.6524390243902439</v>
       </c>
       <c r="I4" t="n">
-        <v>0.375</v>
+        <v>0.5792682926829268</v>
       </c>
       <c r="J4" t="n">
         <v>0.3475609756097561</v>
@@ -636,12 +647,15 @@
         <v>0.5579268292682927</v>
       </c>
       <c r="M4" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.4969512195121951</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>0.399390243902439</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>0.5823170731707317</v>
       </c>
     </row>
@@ -652,7 +666,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2926829268292683</v>
+        <v>0.3170731707317073</v>
       </c>
       <c r="C5" t="n">
         <v>0.625</v>
@@ -673,7 +687,7 @@
         <v>0.5396341463414634</v>
       </c>
       <c r="I5" t="n">
-        <v>0.7530487804878049</v>
+        <v>0.5792682926829268</v>
       </c>
       <c r="J5" t="n">
         <v>0.7957317073170732</v>
@@ -685,12 +699,15 @@
         <v>0.5914634146341463</v>
       </c>
       <c r="M5" t="n">
+        <v>0.7530487804878049</v>
+      </c>
+      <c r="N5" t="n">
         <v>0.676829268292683</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>0.8323170731707317</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>0.6554878048780488</v>
       </c>
     </row>
@@ -701,7 +718,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2835365853658536</v>
+        <v>0.2347560975609756</v>
       </c>
       <c r="C6" t="n">
         <v>0.5701219512195121</v>
@@ -722,7 +739,7 @@
         <v>0.5091463414634146</v>
       </c>
       <c r="I6" t="n">
-        <v>0.75</v>
+        <v>0.5335365853658537</v>
       </c>
       <c r="J6" t="n">
         <v>0.7652439024390244</v>
@@ -734,12 +751,15 @@
         <v>0.573170731707317</v>
       </c>
       <c r="M6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="N6" t="n">
         <v>0.6585365853658537</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>0.8414634146341463</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>0.600609756097561</v>
       </c>
     </row>
@@ -771,7 +791,7 @@
         <v>0.4054878048780488</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7896341463414634</v>
+        <v>0.5030487804878049</v>
       </c>
       <c r="J7" t="n">
         <v>0.8536585365853658</v>
@@ -783,12 +803,15 @@
         <v>0.4969512195121951</v>
       </c>
       <c r="M7" t="n">
+        <v>0.7896341463414634</v>
+      </c>
+      <c r="N7" t="n">
         <v>0.6371951219512195</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>0.7957317073170732</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>0.5945121951219512</v>
       </c>
     </row>
@@ -799,7 +822,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6310975609756098</v>
+        <v>0.6067073170731707</v>
       </c>
       <c r="C8" t="n">
         <v>0.5182926829268293</v>
@@ -820,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4481707317073171</v>
+        <v>0.5640243902439024</v>
       </c>
       <c r="J8" t="n">
         <v>0.4390243902439024</v>
@@ -832,62 +855,68 @@
         <v>0.6371951219512195</v>
       </c>
       <c r="M8" t="n">
+        <v>0.4481707317073171</v>
+      </c>
+      <c r="N8" t="n">
         <v>0.551829268292683</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>0.4603658536585366</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>0.625</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gemeinsame Liste</t>
+          <t>Freie Wähler</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2134146341463415</v>
+        <v>0.6128048780487805</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6341463414634146</v>
+        <v>0.6280487804878049</v>
       </c>
       <c r="D9" t="n">
-        <v>0.375</v>
+        <v>0.5792682926829268</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7530487804878049</v>
+        <v>0.5792682926829268</v>
       </c>
       <c r="F9" t="n">
-        <v>0.75</v>
+        <v>0.5335365853658537</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7896341463414634</v>
+        <v>0.5030487804878049</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4481707317073171</v>
+        <v>0.5640243902439024</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8109756097560976</v>
+        <v>0.5091463414634146</v>
       </c>
       <c r="K9" t="n">
-        <v>0.6158536585365854</v>
+        <v>0.5274390243902439</v>
       </c>
       <c r="L9" t="n">
-        <v>0.5487804878048781</v>
+        <v>0.6219512195121951</v>
       </c>
       <c r="M9" t="n">
+        <v>0.5182926829268293</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.573170731707317</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.5182926829268293</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.6707317073170732</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.8079268292682927</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.600609756097561</v>
       </c>
     </row>
     <row r="10">
@@ -897,7 +926,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2134146341463415</v>
+        <v>0.2378048780487805</v>
       </c>
       <c r="C10" t="n">
         <v>0.6371951219512195</v>
@@ -918,7 +947,7 @@
         <v>0.4390243902439024</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8109756097560976</v>
+        <v>0.5091463414634146</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -930,12 +959,15 @@
         <v>0.5335365853658537</v>
       </c>
       <c r="M10" t="n">
+        <v>0.8109756097560976</v>
+      </c>
+      <c r="N10" t="n">
         <v>0.7012195121951219</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>0.8536585365853658</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>0.6097560975609756</v>
       </c>
     </row>
@@ -946,7 +978,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4390243902439024</v>
+        <v>0.4024390243902439</v>
       </c>
       <c r="C11" t="n">
         <v>0.5335365853658537</v>
@@ -967,7 +999,7 @@
         <v>0.6128048780487805</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6158536585365854</v>
+        <v>0.5274390243902439</v>
       </c>
       <c r="J11" t="n">
         <v>0.6128048780487805</v>
@@ -979,12 +1011,15 @@
         <v>0.6371951219512195</v>
       </c>
       <c r="M11" t="n">
+        <v>0.6158536585365854</v>
+      </c>
+      <c r="N11" t="n">
         <v>0.6615853658536586</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>0.6859756097560976</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>0.6219512195121951</v>
       </c>
     </row>
@@ -1016,7 +1051,7 @@
         <v>0.6371951219512195</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5487804878048781</v>
+        <v>0.6219512195121951</v>
       </c>
       <c r="J12" t="n">
         <v>0.5335365853658537</v>
@@ -1028,159 +1063,223 @@
         <v>1</v>
       </c>
       <c r="M12" t="n">
+        <v>0.5487804878048781</v>
+      </c>
+      <c r="N12" t="n">
         <v>0.6310975609756098</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>0.5335365853658537</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>0.698170731707317</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UFFBASSE</t>
+          <t>Tierschutzpartei</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.423780487804878</v>
+        <v>0.225609756097561</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6615853658536586</v>
+        <v>0.6341463414634146</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4969512195121951</v>
+        <v>0.375</v>
       </c>
       <c r="E13" t="n">
-        <v>0.676829268292683</v>
+        <v>0.7530487804878049</v>
       </c>
       <c r="F13" t="n">
-        <v>0.6585365853658537</v>
+        <v>0.75</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6371951219512195</v>
+        <v>0.7896341463414634</v>
       </c>
       <c r="H13" t="n">
-        <v>0.551829268292683</v>
+        <v>0.4481707317073171</v>
       </c>
       <c r="I13" t="n">
+        <v>0.5182926829268293</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.8109756097560976</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.6158536585365854</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.5487804878048781</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
         <v>0.6707317073170732</v>
       </c>
-      <c r="J13" t="n">
-        <v>0.7012195121951219</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.6615853658536586</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.6310975609756098</v>
-      </c>
-      <c r="M13" t="n">
-        <v>1</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.6737804878048781</v>
-      </c>
       <c r="O13" t="n">
-        <v>0.6646341463414634</v>
+        <v>0.8079268292682927</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.600609756097561</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Volt</t>
+          <t>UFFBASSE</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.2195121951219512</v>
+        <v>0.4481707317073171</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6097560975609756</v>
+        <v>0.6615853658536586</v>
       </c>
       <c r="D14" t="n">
-        <v>0.399390243902439</v>
+        <v>0.4969512195121951</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8323170731707317</v>
+        <v>0.676829268292683</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8414634146341463</v>
+        <v>0.6585365853658537</v>
       </c>
       <c r="G14" t="n">
-        <v>0.7957317073170732</v>
+        <v>0.6371951219512195</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4603658536585366</v>
+        <v>0.551829268292683</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8079268292682927</v>
+        <v>0.573170731707317</v>
       </c>
       <c r="J14" t="n">
-        <v>0.8536585365853658</v>
+        <v>0.7012195121951219</v>
       </c>
       <c r="K14" t="n">
-        <v>0.6859756097560976</v>
+        <v>0.6615853658536586</v>
       </c>
       <c r="L14" t="n">
-        <v>0.5335365853658537</v>
+        <v>0.6310975609756098</v>
       </c>
       <c r="M14" t="n">
+        <v>0.6707317073170732</v>
+      </c>
+      <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
         <v>0.6737804878048781</v>
       </c>
-      <c r="N14" t="n">
-        <v>1</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0.5975609756097561</v>
+      <c r="P14" t="n">
+        <v>0.6646341463414634</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Volt</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.2195121951219512</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.6097560975609756</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.399390243902439</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.8323170731707317</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.8414634146341463</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.7957317073170732</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.4603658536585366</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.5182926829268293</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.8536585365853658</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.6859756097560976</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.5335365853658537</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.8079268292682927</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.6737804878048781</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.5975609756097561</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>WGD</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>0.4695121951219512</v>
-      </c>
-      <c r="C15" t="n">
+      <c r="B16" t="n">
+        <v>0.4939024390243902</v>
+      </c>
+      <c r="C16" t="n">
         <v>0.6280487804878049</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" t="n">
         <v>0.5823170731707317</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E16" t="n">
         <v>0.6554878048780488</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F16" t="n">
         <v>0.600609756097561</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G16" t="n">
         <v>0.5945121951219512</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H16" t="n">
         <v>0.625</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I16" t="n">
+        <v>0.6707317073170732</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.6097560975609756</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.6219512195121951</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.698170731707317</v>
+      </c>
+      <c r="M16" t="n">
         <v>0.600609756097561</v>
       </c>
-      <c r="J15" t="n">
-        <v>0.6097560975609756</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.6219512195121951</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.698170731707317</v>
-      </c>
-      <c r="M15" t="n">
+      <c r="N16" t="n">
         <v>0.6646341463414634</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O16" t="n">
         <v>0.5975609756097561</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P16" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>